<commit_message>
delete comment in template
</commit_message>
<xml_diff>
--- a/bin/templates/DailyReport-v2.xlsx
+++ b/bin/templates/DailyReport-v2.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17571"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jerick\Desktop\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4507"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="9660" windowHeight="5490"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="9660" windowHeight="5496"/>
   </bookViews>
   <sheets>
     <sheet name="DailyProductionReport" sheetId="1" r:id="rId1"/>
@@ -18,216 +13,8 @@
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">DailyProductionReport!$1:$1</definedName>
   </definedNames>
-  <calcPr calcId="171027" fullCalcOnLoad="1"/>
+  <calcPr calcId="125725"/>
 </workbook>
-</file>
-
-<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <authors>
-    <author>Jerick</author>
-  </authors>
-  <commentList>
-    <comment ref="C10" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Jerick:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Incorrect COD dates.
-I have corrected it here</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="F10" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Jerick:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Incorrect Monthly Budget</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="G10" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Jerick:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Incorrect IE POA Insolation.  
-I corrected it here.
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="H10" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Jerick:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-This should accumulate the daily insolation</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="I10" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Jerick:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Accumulate the daily production
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="M10" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Jerick:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-This should be reference to:
-Total Energy/Monthly Budget</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="N10" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Jerick:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Change Formula to:
-Total Energy/(Monthly Budget kWH x Weather Performance %)</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="O10" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Jerick:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Total Insolation/IE POA Insolation</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
@@ -398,14 +185,14 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="164" formatCode="[$-10409]#,##0;\(#,##0\)"/>
     <numFmt numFmtId="165" formatCode="[$-10409]0%"/>
     <numFmt numFmtId="166" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
     <numFmt numFmtId="167" formatCode="[$-10409]#,##0.00;\(#,##0.00\)"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -448,19 +235,6 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
       <b/>
       <sz val="8"/>
       <color indexed="9"/>
@@ -961,104 +735,104 @@
       <alignment vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="167" fontId="4" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="167" fontId="4" fillId="2" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="167" fontId="4" fillId="2" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="167" fontId="4" fillId="4" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="167" fontId="4" fillId="4" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="167" fontId="4" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="167" fontId="4" fillId="2" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="167" fontId="4" fillId="2" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="167" fontId="4" fillId="4" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="167" fontId="4" fillId="4" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -1121,7 +895,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -1173,7 +947,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -1367,52 +1141,52 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:O15"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScaleNormal="100" zoomScalePageLayoutView="145" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="G24" sqref="G24"/>
+      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.5" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.45" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="17.08984375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="25.26953125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="21.26953125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="17.109375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="25.21875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="21.21875" style="2" customWidth="1"/>
     <col min="4" max="9" width="13" style="2" customWidth="1"/>
-    <col min="10" max="13" width="19.1796875" style="2" customWidth="1"/>
+    <col min="10" max="13" width="19.21875" style="2" customWidth="1"/>
     <col min="14" max="15" width="21" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="43" t="s">
+    <row r="1" spans="1:15" ht="28.5" customHeight="1">
+      <c r="A1" s="58" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="43"/>
-      <c r="C1" s="43"/>
-      <c r="D1" s="43"/>
-      <c r="E1" s="43"/>
-      <c r="F1" s="43"/>
-      <c r="G1" s="43"/>
-      <c r="H1" s="43"/>
-      <c r="I1" s="43"/>
-      <c r="J1" s="43"/>
-      <c r="K1" s="43"/>
-      <c r="L1" s="43"/>
-      <c r="M1" s="43"/>
-      <c r="N1" s="43"/>
-      <c r="O1" s="43"/>
-    </row>
-    <row r="2" spans="1:15" ht="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="58"/>
+      <c r="C1" s="58"/>
+      <c r="D1" s="58"/>
+      <c r="E1" s="58"/>
+      <c r="F1" s="58"/>
+      <c r="G1" s="58"/>
+      <c r="H1" s="58"/>
+      <c r="I1" s="58"/>
+      <c r="J1" s="58"/>
+      <c r="K1" s="58"/>
+      <c r="L1" s="58"/>
+      <c r="M1" s="58"/>
+      <c r="N1" s="58"/>
+      <c r="O1" s="58"/>
+    </row>
+    <row r="2" spans="1:15" ht="1.05" customHeight="1"/>
+    <row r="3" spans="1:15" ht="15.75" customHeight="1">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -1420,51 +1194,51 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" ht="15.75" customHeight="1">
       <c r="B4" s="4"/>
     </row>
-    <row r="5" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="43" t="s">
+    <row r="5" spans="1:15" ht="18" customHeight="1">
+      <c r="A5" s="58" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="43"/>
-      <c r="C5" s="43"/>
-      <c r="D5" s="43"/>
-      <c r="E5" s="43"/>
+      <c r="B5" s="58"/>
+      <c r="C5" s="58"/>
+      <c r="D5" s="58"/>
+      <c r="E5" s="58"/>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
     </row>
-    <row r="6" spans="1:15" ht="2.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="7" spans="1:15" s="10" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:15" ht="2.7" customHeight="1" thickBot="1"/>
+    <row r="7" spans="1:15" s="10" customFormat="1" ht="22.5" customHeight="1" thickBot="1">
       <c r="A7" s="11"/>
       <c r="B7" s="23"/>
       <c r="C7" s="31"/>
       <c r="D7" s="26"/>
       <c r="E7" s="27"/>
-      <c r="F7" s="53" t="s">
+      <c r="F7" s="59" t="s">
         <v>50</v>
       </c>
-      <c r="G7" s="54"/>
-      <c r="H7" s="53" t="s">
+      <c r="G7" s="60"/>
+      <c r="H7" s="59" t="s">
         <v>48</v>
       </c>
-      <c r="I7" s="54"/>
-      <c r="J7" s="60" t="s">
+      <c r="I7" s="60"/>
+      <c r="J7" s="54" t="s">
         <v>51</v>
       </c>
-      <c r="K7" s="41"/>
+      <c r="K7" s="55"/>
       <c r="L7" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="M7" s="61" t="s">
+      <c r="M7" s="56" t="s">
         <v>52</v>
       </c>
-      <c r="N7" s="42"/>
-      <c r="O7" s="42"/>
-    </row>
-    <row r="8" spans="1:15" s="3" customFormat="1" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="N7" s="57"/>
+      <c r="O7" s="57"/>
+    </row>
+    <row r="8" spans="1:15" s="3" customFormat="1" ht="12.45" customHeight="1">
       <c r="A8" s="12" t="s">
         <v>7</v>
       </c>
@@ -1474,20 +1248,20 @@
       <c r="C8" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="D8" s="38" t="s">
+      <c r="D8" s="52" t="s">
         <v>10</v>
       </c>
-      <c r="E8" s="44"/>
-      <c r="F8" s="46" t="s">
+      <c r="E8" s="53"/>
+      <c r="F8" s="39" t="s">
         <v>45</v>
       </c>
-      <c r="G8" s="50" t="s">
+      <c r="G8" s="43" t="s">
         <v>15</v>
       </c>
-      <c r="H8" s="55" t="s">
+      <c r="H8" s="46" t="s">
         <v>49</v>
       </c>
-      <c r="I8" s="47" t="s">
+      <c r="I8" s="40" t="s">
         <v>53</v>
       </c>
       <c r="J8" s="8" t="s">
@@ -1509,7 +1283,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:15" s="30" customFormat="1" ht="12.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:15" s="30" customFormat="1" ht="12.45" customHeight="1">
       <c r="A9" s="28"/>
       <c r="B9" s="5"/>
       <c r="C9" s="9"/>
@@ -1519,22 +1293,22 @@
       <c r="E9" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="F9" s="48" t="s">
+      <c r="F9" s="41" t="s">
         <v>22</v>
       </c>
-      <c r="G9" s="51" t="s">
+      <c r="G9" s="44" t="s">
         <v>23</v>
       </c>
-      <c r="H9" s="56" t="s">
+      <c r="H9" s="47" t="s">
         <v>23</v>
       </c>
-      <c r="I9" s="57" t="s">
+      <c r="I9" s="48" t="s">
         <v>22</v>
       </c>
       <c r="J9" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="K9" s="62" t="s">
+      <c r="K9" s="51" t="s">
         <v>22</v>
       </c>
       <c r="L9" s="28" t="s">
@@ -1550,7 +1324,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:15" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" ht="12.45" customHeight="1">
       <c r="A10" s="14">
         <v>1</v>
       </c>
@@ -1563,17 +1337,17 @@
       <c r="D10" s="35">
         <v>450</v>
       </c>
-      <c r="E10" s="45">
+      <c r="E10" s="38">
         <v>653</v>
       </c>
-      <c r="F10" s="49">
+      <c r="F10" s="42">
         <v>25730.243009613656</v>
       </c>
-      <c r="G10" s="52">
+      <c r="G10" s="45">
         <v>58.4</v>
       </c>
-      <c r="H10" s="58"/>
-      <c r="I10" s="59"/>
+      <c r="H10" s="49"/>
+      <c r="I10" s="50"/>
       <c r="J10" s="7">
         <f>L10/G10*F10</f>
         <v>590.38571289182028</v>
@@ -1594,7 +1368,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="1:15" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" ht="12.45" customHeight="1">
       <c r="A11" s="14">
         <v>2</v>
       </c>
@@ -1607,17 +1381,17 @@
       <c r="D11" s="35">
         <v>150</v>
       </c>
-      <c r="E11" s="45">
+      <c r="E11" s="38">
         <v>162.69999999999999</v>
       </c>
-      <c r="F11" s="49">
+      <c r="F11" s="42">
         <v>6300.8349248068307</v>
       </c>
-      <c r="G11" s="52">
+      <c r="G11" s="45">
         <v>48.5</v>
       </c>
-      <c r="H11" s="58"/>
-      <c r="I11" s="59"/>
+      <c r="H11" s="49"/>
+      <c r="I11" s="50"/>
       <c r="J11" s="7">
         <f t="shared" ref="J11:J14" si="0">L11/G11*F11</f>
         <v>167.58921758764561</v>
@@ -1638,7 +1412,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="12" spans="1:15" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" ht="12.45" customHeight="1">
       <c r="A12" s="14">
         <v>3</v>
       </c>
@@ -1651,17 +1425,17 @@
       <c r="D12" s="35">
         <v>500</v>
       </c>
-      <c r="E12" s="45">
+      <c r="E12" s="38">
         <v>602.91</v>
       </c>
-      <c r="F12" s="49">
+      <c r="F12" s="42">
         <v>19776.504839953755</v>
       </c>
-      <c r="G12" s="52">
+      <c r="G12" s="45">
         <v>57.3</v>
       </c>
-      <c r="H12" s="58"/>
-      <c r="I12" s="59"/>
+      <c r="H12" s="49"/>
+      <c r="I12" s="50"/>
       <c r="J12" s="7">
         <f t="shared" si="0"/>
         <v>414.1676406273038</v>
@@ -1678,7 +1452,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="13" spans="1:15" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" ht="12.45" customHeight="1">
       <c r="A13" s="14">
         <v>4</v>
       </c>
@@ -1691,17 +1465,17 @@
       <c r="D13" s="35">
         <v>250</v>
       </c>
-      <c r="E13" s="45">
+      <c r="E13" s="38">
         <v>306.24</v>
       </c>
-      <c r="F13" s="49">
+      <c r="F13" s="42">
         <v>12488.748804436693</v>
       </c>
-      <c r="G13" s="52">
+      <c r="G13" s="45">
         <v>58.1</v>
       </c>
-      <c r="H13" s="58"/>
-      <c r="I13" s="59"/>
+      <c r="H13" s="49"/>
+      <c r="I13" s="50"/>
       <c r="J13" s="7">
         <f t="shared" si="0"/>
         <v>255.79365021135391</v>
@@ -1722,7 +1496,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="14" spans="1:15" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" ht="12.45" customHeight="1">
       <c r="A14" s="14">
         <v>5</v>
       </c>
@@ -1735,17 +1509,17 @@
       <c r="D14" s="35">
         <v>500</v>
       </c>
-      <c r="E14" s="45">
+      <c r="E14" s="38">
         <v>611.29999999999995</v>
       </c>
-      <c r="F14" s="49">
+      <c r="F14" s="42">
         <v>24402.408882923904</v>
       </c>
-      <c r="G14" s="52">
+      <c r="G14" s="45">
         <v>61.2</v>
       </c>
-      <c r="H14" s="58"/>
-      <c r="I14" s="59"/>
+      <c r="H14" s="49"/>
+      <c r="I14" s="50"/>
       <c r="J14" s="7">
         <f t="shared" si="0"/>
         <v>311.01109360589288</v>
@@ -1762,7 +1536,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="15" spans="1:15" ht="13" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:15" ht="13.05" customHeight="1" thickBot="1">
       <c r="A15" s="24"/>
       <c r="B15" s="25" t="s">
         <v>41</v>
@@ -1824,48 +1598,47 @@
     <oddFooter xml:space="preserve">&amp;L&amp;"Arial"&amp;8&amp;Iv1.0&amp;I 
 &amp;I© 2017 SunEdison&amp;I &amp;C&amp;R&amp;"Arial"&amp;8 Page 1 of 2 </oddFooter>
   </headerFooter>
-  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:N15"/>
   <sheetViews>
     <sheetView showRuler="0" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D10" sqref="D10:E14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.5" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.45" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="17.08984375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="25.26953125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="21.26953125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="17.109375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="25.21875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="21.21875" style="2" customWidth="1"/>
     <col min="4" max="5" width="13" style="2" customWidth="1"/>
-    <col min="6" max="11" width="19.1796875" style="2" customWidth="1"/>
+    <col min="6" max="11" width="19.21875" style="2" customWidth="1"/>
     <col min="12" max="14" width="21" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="43" t="s">
+    <row r="1" spans="1:14" ht="28.5" customHeight="1">
+      <c r="A1" s="58" t="s">
         <v>42</v>
       </c>
-      <c r="B1" s="43"/>
-      <c r="C1" s="43"/>
-      <c r="D1" s="43"/>
-      <c r="E1" s="43"/>
-      <c r="F1" s="43"/>
-      <c r="G1" s="43"/>
-      <c r="H1" s="43"/>
-      <c r="I1" s="43"/>
-      <c r="J1" s="43"/>
-      <c r="K1" s="43"/>
-      <c r="L1" s="43"/>
-      <c r="M1" s="43"/>
-      <c r="N1" s="43"/>
-    </row>
-    <row r="2" spans="1:14" ht="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="58"/>
+      <c r="C1" s="58"/>
+      <c r="D1" s="58"/>
+      <c r="E1" s="58"/>
+      <c r="F1" s="58"/>
+      <c r="G1" s="58"/>
+      <c r="H1" s="58"/>
+      <c r="I1" s="58"/>
+      <c r="J1" s="58"/>
+      <c r="K1" s="58"/>
+      <c r="L1" s="58"/>
+      <c r="M1" s="58"/>
+      <c r="N1" s="58"/>
+    </row>
+    <row r="2" spans="1:14" ht="1.05" customHeight="1"/>
+    <row r="3" spans="1:14" ht="15.75" customHeight="1">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -1873,42 +1646,42 @@
         <v>42794</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" ht="15.75" customHeight="1">
       <c r="B4" s="4"/>
     </row>
-    <row r="5" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="43" t="s">
+    <row r="5" spans="1:14" ht="18" customHeight="1">
+      <c r="A5" s="58" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="43"/>
-      <c r="C5" s="43"/>
-      <c r="D5" s="43"/>
-      <c r="E5" s="43"/>
-    </row>
-    <row r="6" spans="1:14" ht="2.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="7" spans="1:14" s="10" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="58"/>
+      <c r="C5" s="58"/>
+      <c r="D5" s="58"/>
+      <c r="E5" s="58"/>
+    </row>
+    <row r="6" spans="1:14" ht="2.7" customHeight="1"/>
+    <row r="7" spans="1:14" s="10" customFormat="1" ht="22.5" customHeight="1">
       <c r="A7" s="11"/>
       <c r="B7" s="23"/>
       <c r="C7" s="31"/>
       <c r="D7" s="26"/>
       <c r="E7" s="27"/>
-      <c r="F7" s="40" t="s">
+      <c r="F7" s="61" t="s">
         <v>4</v>
       </c>
-      <c r="G7" s="42"/>
-      <c r="H7" s="41"/>
-      <c r="I7" s="40" t="s">
+      <c r="G7" s="57"/>
+      <c r="H7" s="55"/>
+      <c r="I7" s="61" t="s">
         <v>5</v>
       </c>
-      <c r="J7" s="41"/>
-      <c r="K7" s="40" t="s">
+      <c r="J7" s="55"/>
+      <c r="K7" s="61" t="s">
         <v>6</v>
       </c>
-      <c r="L7" s="42"/>
-      <c r="M7" s="42"/>
-      <c r="N7" s="41"/>
-    </row>
-    <row r="8" spans="1:14" s="3" customFormat="1" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L7" s="57"/>
+      <c r="M7" s="57"/>
+      <c r="N7" s="55"/>
+    </row>
+    <row r="8" spans="1:14" s="3" customFormat="1" ht="12.45" customHeight="1">
       <c r="A8" s="12" t="s">
         <v>7</v>
       </c>
@@ -1918,10 +1691,10 @@
       <c r="C8" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="D8" s="38" t="s">
+      <c r="D8" s="52" t="s">
         <v>10</v>
       </c>
-      <c r="E8" s="39"/>
+      <c r="E8" s="62"/>
       <c r="F8" s="12" t="s">
         <v>11</v>
       </c>
@@ -1950,7 +1723,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="9" spans="1:14" s="30" customFormat="1" ht="12.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14" s="30" customFormat="1" ht="12.45" customHeight="1">
       <c r="A9" s="28"/>
       <c r="B9" s="5"/>
       <c r="C9" s="9"/>
@@ -1988,7 +1761,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" ht="12.45" customHeight="1">
       <c r="A10" s="14">
         <v>1</v>
       </c>
@@ -2016,7 +1789,7 @@
       <c r="M10" s="7"/>
       <c r="N10" s="20"/>
     </row>
-    <row r="11" spans="1:14" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" ht="12.45" customHeight="1">
       <c r="A11" s="14">
         <v>2</v>
       </c>
@@ -2044,7 +1817,7 @@
       <c r="M11" s="7"/>
       <c r="N11" s="20"/>
     </row>
-    <row r="12" spans="1:14" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" ht="12.45" customHeight="1">
       <c r="A12" s="14">
         <v>3</v>
       </c>
@@ -2072,7 +1845,7 @@
       <c r="M12" s="7"/>
       <c r="N12" s="20"/>
     </row>
-    <row r="13" spans="1:14" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" ht="12.45" customHeight="1">
       <c r="A13" s="14">
         <v>4</v>
       </c>
@@ -2100,7 +1873,7 @@
       <c r="M13" s="7"/>
       <c r="N13" s="21"/>
     </row>
-    <row r="14" spans="1:14" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" ht="12.45" customHeight="1">
       <c r="A14" s="14">
         <v>5</v>
       </c>
@@ -2126,7 +1899,7 @@
       <c r="M14" s="7"/>
       <c r="N14" s="21"/>
     </row>
-    <row r="15" spans="1:14" ht="13" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" ht="13.05" customHeight="1">
       <c r="A15" s="24"/>
       <c r="B15" s="25" t="s">
         <v>41</v>
@@ -2167,12 +1940,12 @@
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="D8:E8"/>
     <mergeCell ref="A1:N1"/>
     <mergeCell ref="A5:E5"/>
     <mergeCell ref="F7:H7"/>
     <mergeCell ref="I7:J7"/>
     <mergeCell ref="K7:N7"/>
-    <mergeCell ref="D8:E8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>

</xml_diff>

<commit_message>
suffix filename with user id
</commit_message>
<xml_diff>
--- a/bin/templates/DailyReport-v2.xlsx
+++ b/bin/templates/DailyReport-v2.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="43">
   <si>
     <t>Daily Solar Energy Production Report</t>
   </si>
@@ -98,49 +98,16 @@
     <t>125 Bermondsey</t>
   </si>
   <si>
-    <t>1.03%</t>
-  </si>
-  <si>
-    <t>31.85%</t>
-  </si>
-  <si>
-    <t>3.23%</t>
-  </si>
-  <si>
     <t>1935 Drew</t>
   </si>
   <si>
-    <t>1.79%</t>
-  </si>
-  <si>
-    <t>56.6%</t>
-  </si>
-  <si>
-    <t>3.17%</t>
-  </si>
-  <si>
     <t>1755 Brimley</t>
   </si>
   <si>
-    <t>2.83%</t>
-  </si>
-  <si>
     <t>200 Bullock</t>
   </si>
   <si>
-    <t>0.45%</t>
-  </si>
-  <si>
-    <t>16.06%</t>
-  </si>
-  <si>
-    <t>2.82%</t>
-  </si>
-  <si>
     <t>51 Gerry Fitzgerald</t>
-  </si>
-  <si>
-    <t>1.89%</t>
   </si>
   <si>
     <t>TOTAL:</t>
@@ -827,12 +794,12 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -1141,7 +1108,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1153,7 +1120,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScaleNormal="100" zoomScalePageLayoutView="145" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
+      <selection pane="bottomLeft" activeCell="O10" sqref="O10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.45" customHeight="1"/>
@@ -1218,22 +1185,22 @@
       <c r="D7" s="26"/>
       <c r="E7" s="27"/>
       <c r="F7" s="59" t="s">
-        <v>50</v>
+        <v>39</v>
       </c>
       <c r="G7" s="60"/>
       <c r="H7" s="59" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="I7" s="60"/>
       <c r="J7" s="54" t="s">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="K7" s="55"/>
       <c r="L7" s="11" t="s">
         <v>5</v>
       </c>
       <c r="M7" s="56" t="s">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="N7" s="57"/>
       <c r="O7" s="57"/>
@@ -1253,22 +1220,22 @@
       </c>
       <c r="E8" s="53"/>
       <c r="F8" s="39" t="s">
-        <v>45</v>
+        <v>34</v>
       </c>
       <c r="G8" s="43" t="s">
         <v>15</v>
       </c>
       <c r="H8" s="46" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
       <c r="I8" s="40" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="J8" s="8" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="K8" s="13" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="L8" s="12" t="s">
         <v>14</v>
@@ -1325,258 +1292,131 @@
       </c>
     </row>
     <row r="10" spans="1:15" ht="12.45" customHeight="1">
-      <c r="A10" s="14">
-        <v>1</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="C10" s="33">
-        <v>41384</v>
-      </c>
-      <c r="D10" s="35">
-        <v>450</v>
-      </c>
-      <c r="E10" s="38">
-        <v>653</v>
-      </c>
-      <c r="F10" s="42">
-        <v>25730.243009613656</v>
-      </c>
-      <c r="G10" s="45">
-        <v>58.4</v>
-      </c>
+      <c r="A10" s="14"/>
+      <c r="B10" s="6"/>
+      <c r="C10" s="33"/>
+      <c r="D10" s="35"/>
+      <c r="E10" s="38"/>
+      <c r="F10" s="42"/>
+      <c r="G10" s="45"/>
       <c r="H10" s="49"/>
       <c r="I10" s="50"/>
-      <c r="J10" s="7">
-        <f>L10/G10*F10</f>
-        <v>590.38571289182028</v>
-      </c>
-      <c r="K10" s="16">
-        <v>376.73</v>
-      </c>
-      <c r="L10" s="15">
-        <v>1.34</v>
-      </c>
-      <c r="M10" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="N10" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="O10" s="7" t="s">
-        <v>28</v>
-      </c>
+      <c r="J10" s="7"/>
+      <c r="K10" s="16"/>
+      <c r="L10" s="15"/>
+      <c r="M10" s="15"/>
+      <c r="N10" s="7"/>
+      <c r="O10" s="7"/>
     </row>
     <row r="11" spans="1:15" ht="12.45" customHeight="1">
-      <c r="A11" s="14">
-        <v>2</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="C11" s="33">
-        <v>41312</v>
-      </c>
-      <c r="D11" s="35">
-        <v>150</v>
-      </c>
-      <c r="E11" s="38">
-        <v>162.69999999999999</v>
-      </c>
-      <c r="F11" s="42">
-        <v>6300.8349248068307</v>
-      </c>
-      <c r="G11" s="45">
-        <v>48.5</v>
-      </c>
+      <c r="A11" s="14"/>
+      <c r="B11" s="6"/>
+      <c r="C11" s="33"/>
+      <c r="D11" s="35"/>
+      <c r="E11" s="38"/>
+      <c r="F11" s="42"/>
+      <c r="G11" s="45"/>
       <c r="H11" s="49"/>
       <c r="I11" s="50"/>
-      <c r="J11" s="7">
-        <f t="shared" ref="J11:J14" si="0">L11/G11*F11</f>
-        <v>167.58921758764561</v>
-      </c>
-      <c r="K11" s="16">
-        <v>159.87</v>
-      </c>
-      <c r="L11" s="15">
-        <v>1.29</v>
-      </c>
-      <c r="M11" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="N11" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="O11" s="7" t="s">
-        <v>32</v>
-      </c>
+      <c r="J11" s="7"/>
+      <c r="K11" s="16"/>
+      <c r="L11" s="15"/>
+      <c r="M11" s="15"/>
+      <c r="N11" s="7"/>
+      <c r="O11" s="7"/>
     </row>
     <row r="12" spans="1:15" ht="12.45" customHeight="1">
-      <c r="A12" s="14">
-        <v>3</v>
-      </c>
-      <c r="B12" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="C12" s="33">
-        <v>41537</v>
-      </c>
-      <c r="D12" s="35">
-        <v>500</v>
-      </c>
-      <c r="E12" s="38">
-        <v>602.91</v>
-      </c>
-      <c r="F12" s="42">
-        <v>19776.504839953755</v>
-      </c>
-      <c r="G12" s="45">
-        <v>57.3</v>
-      </c>
+      <c r="A12" s="14"/>
+      <c r="B12" s="6"/>
+      <c r="C12" s="33"/>
+      <c r="D12" s="35"/>
+      <c r="E12" s="38"/>
+      <c r="F12" s="42"/>
+      <c r="G12" s="45"/>
       <c r="H12" s="49"/>
       <c r="I12" s="50"/>
-      <c r="J12" s="7">
-        <f t="shared" si="0"/>
-        <v>414.1676406273038</v>
-      </c>
-      <c r="K12" s="16">
-        <v>87.67</v>
-      </c>
-      <c r="L12" s="15">
-        <v>1.2</v>
-      </c>
+      <c r="J12" s="7"/>
+      <c r="K12" s="16"/>
+      <c r="L12" s="15"/>
       <c r="M12" s="15"/>
       <c r="N12" s="7"/>
-      <c r="O12" s="7" t="s">
-        <v>34</v>
-      </c>
+      <c r="O12" s="7"/>
     </row>
     <row r="13" spans="1:15" ht="12.45" customHeight="1">
-      <c r="A13" s="14">
-        <v>4</v>
-      </c>
-      <c r="B13" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="C13" s="33">
-        <v>41529</v>
-      </c>
-      <c r="D13" s="35">
-        <v>250</v>
-      </c>
-      <c r="E13" s="38">
-        <v>306.24</v>
-      </c>
-      <c r="F13" s="42">
-        <v>12488.748804436693</v>
-      </c>
-      <c r="G13" s="45">
-        <v>58.1</v>
-      </c>
+      <c r="A13" s="14"/>
+      <c r="B13" s="6"/>
+      <c r="C13" s="33"/>
+      <c r="D13" s="35"/>
+      <c r="E13" s="38"/>
+      <c r="F13" s="42"/>
+      <c r="G13" s="45"/>
       <c r="H13" s="49"/>
       <c r="I13" s="50"/>
-      <c r="J13" s="7">
-        <f t="shared" si="0"/>
-        <v>255.79365021135391</v>
-      </c>
-      <c r="K13" s="16">
-        <v>80.62</v>
-      </c>
-      <c r="L13" s="15">
-        <v>1.19</v>
-      </c>
-      <c r="M13" s="15" t="s">
-        <v>36</v>
-      </c>
-      <c r="N13" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="O13" s="7" t="s">
-        <v>38</v>
-      </c>
+      <c r="J13" s="7"/>
+      <c r="K13" s="16"/>
+      <c r="L13" s="15"/>
+      <c r="M13" s="15"/>
+      <c r="N13" s="7"/>
+      <c r="O13" s="7"/>
     </row>
     <row r="14" spans="1:15" ht="12.45" customHeight="1">
-      <c r="A14" s="14">
-        <v>5</v>
-      </c>
-      <c r="B14" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="C14" s="33">
-        <v>41537</v>
-      </c>
-      <c r="D14" s="35">
-        <v>500</v>
-      </c>
-      <c r="E14" s="38">
-        <v>611.29999999999995</v>
-      </c>
-      <c r="F14" s="42">
-        <v>24402.408882923904</v>
-      </c>
-      <c r="G14" s="45">
-        <v>61.2</v>
-      </c>
+      <c r="A14" s="14"/>
+      <c r="B14" s="6"/>
+      <c r="C14" s="33"/>
+      <c r="D14" s="35"/>
+      <c r="E14" s="38"/>
+      <c r="F14" s="42"/>
+      <c r="G14" s="45"/>
       <c r="H14" s="49"/>
       <c r="I14" s="50"/>
-      <c r="J14" s="7">
-        <f t="shared" si="0"/>
-        <v>311.01109360589288</v>
-      </c>
-      <c r="K14" s="16">
-        <v>630.49</v>
-      </c>
-      <c r="L14" s="15">
-        <v>0.78</v>
-      </c>
+      <c r="J14" s="7"/>
+      <c r="K14" s="16"/>
+      <c r="L14" s="15"/>
       <c r="M14" s="15"/>
       <c r="N14" s="7"/>
-      <c r="O14" s="7" t="s">
-        <v>40</v>
-      </c>
+      <c r="O14" s="7"/>
     </row>
     <row r="15" spans="1:15" ht="13.05" customHeight="1" thickBot="1">
       <c r="A15" s="24"/>
       <c r="B15" s="25" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="C15" s="34"/>
       <c r="D15" s="17">
         <f>SUM(D10:D14)</f>
-        <v>1850</v>
+        <v>0</v>
       </c>
       <c r="E15" s="17">
-        <f t="shared" ref="E15:L15" si="1">SUM(E10:E14)</f>
-        <v>2336.15</v>
+        <f t="shared" ref="E15:L15" si="0">SUM(E10:E14)</f>
+        <v>0</v>
       </c>
       <c r="F15" s="17">
-        <f t="shared" si="1"/>
-        <v>88698.740461734837</v>
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
       <c r="G15" s="17">
-        <f t="shared" si="1"/>
-        <v>283.5</v>
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
       <c r="H15" s="17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="I15" s="17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="J15" s="17">
-        <f t="shared" si="1"/>
-        <v>1738.9473149240166</v>
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
       <c r="K15" s="17">
-        <f t="shared" si="1"/>
-        <v>1335.38</v>
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
       <c r="L15" s="17">
-        <f t="shared" si="1"/>
-        <v>5.8</v>
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
       <c r="M15" s="17"/>
       <c r="N15" s="18"/>
@@ -1621,7 +1461,7 @@
   <sheetData>
     <row r="1" spans="1:14" ht="28.5" customHeight="1">
       <c r="A1" s="58" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
       <c r="B1" s="58"/>
       <c r="C1" s="58"/>
@@ -1665,16 +1505,16 @@
       <c r="C7" s="31"/>
       <c r="D7" s="26"/>
       <c r="E7" s="27"/>
-      <c r="F7" s="61" t="s">
+      <c r="F7" s="62" t="s">
         <v>4</v>
       </c>
       <c r="G7" s="57"/>
       <c r="H7" s="55"/>
-      <c r="I7" s="61" t="s">
+      <c r="I7" s="62" t="s">
         <v>5</v>
       </c>
       <c r="J7" s="55"/>
-      <c r="K7" s="61" t="s">
+      <c r="K7" s="62" t="s">
         <v>6</v>
       </c>
       <c r="L7" s="57"/>
@@ -1694,7 +1534,7 @@
       <c r="D8" s="52" t="s">
         <v>10</v>
       </c>
-      <c r="E8" s="62"/>
+      <c r="E8" s="61"/>
       <c r="F8" s="12" t="s">
         <v>11</v>
       </c>
@@ -1720,7 +1560,7 @@
         <v>18</v>
       </c>
       <c r="N8" s="13" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:14" s="30" customFormat="1" ht="12.45" customHeight="1">
@@ -1758,7 +1598,7 @@
         <v>24</v>
       </c>
       <c r="N9" s="29" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
     </row>
     <row r="10" spans="1:14" ht="12.45" customHeight="1">
@@ -1766,7 +1606,7 @@
         <v>1</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C10" s="33">
         <v>41312</v>
@@ -1822,7 +1662,7 @@
         <v>3</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="C12" s="33">
         <v>41544</v>
@@ -1850,7 +1690,7 @@
         <v>4</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="C13" s="33">
         <v>41529</v>
@@ -1878,7 +1718,7 @@
         <v>5</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="C14" s="33">
         <v>41537</v>
@@ -1902,7 +1742,7 @@
     <row r="15" spans="1:14" ht="13.05" customHeight="1">
       <c r="A15" s="24"/>
       <c r="B15" s="25" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="C15" s="34"/>
       <c r="D15" s="17">

</xml_diff>